<commit_message>
text in graphics changes mainly
</commit_message>
<xml_diff>
--- a/input/translation_asylumFlowsEU.xlsx
+++ b/input/translation_asylumFlowsEU.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="258">
   <si>
     <t>code</t>
   </si>
@@ -76,6 +76,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>- </t>
     </r>
@@ -84,6 +85,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>البلدان الأصلية والوجهات </t>
     </r>
@@ -106,6 +108,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>-</t>
     </r>
@@ -114,6 +117,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>来源国与目的地国</t>
     </r>
@@ -145,6 +149,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>. </t>
     </r>
@@ -153,6 +158,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>حينما يكون الربط بين بلدان المقصد وبلدان المنشأ عن طريق شرائط سميكة، فذلك يعني أنها سجّلت توافد عدد أكبر من طالبي اللجوء مقارنة بالبلدان المرتبطة بشرائط أرقّ</t>
     </r>
@@ -161,6 +167,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>. </t>
     </r>
@@ -237,6 +244,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>. </t>
     </r>
@@ -245,6 +253,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>إذا كنت تنتقل عبر الدول </t>
     </r>
@@ -253,6 +262,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>(</t>
     </r>
@@ -261,6 +271,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>في الأعلى أو في الأسفل</t>
     </r>
@@ -269,6 +280,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>) </t>
     </r>
@@ -277,6 +289,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>بالفأرة، سترى إجمالي عدد طلبات اللجوء حسب البلد وما تمثله من نسبة مائوية من إجمالي الطلبات</t>
     </r>
@@ -285,6 +298,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>. </t>
     </r>
@@ -293,6 +307,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>إذا قمت بتحريك الفأرة فوق أحد الأشرطة، سترى عدد طلبات اللجوء حسب بلد المنشأ والمقصد</t>
     </r>
@@ -301,6 +316,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>. </t>
     </r>
@@ -309,6 +325,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>يُمكن أيضا إعادة ترتيب الدول من خلال النقر أو الإمساك أو السّحب</t>
     </r>
@@ -317,6 +334,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>. </t>
     </r>
@@ -325,6 +343,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>كما يُمكن إعادة ترتيبها أبجديا </t>
     </r>
@@ -333,6 +352,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>(</t>
     </r>
@@ -341,6 +361,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>عن طريق النقر على </t>
     </r>
@@ -349,6 +370,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>'alpha')</t>
     </r>
@@ -357,6 +379,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>، أو حسب الحجم </t>
     </r>
@@ -365,6 +388,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>(</t>
     </r>
@@ -373,6 +397,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>بالنقر على </t>
     </r>
@@ -381,6 +406,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>'size').</t>
     </r>
@@ -400,6 +426,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>alpha</t>
     </r>
@@ -408,6 +435,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>」をクリックするとアルファベット順に、「</t>
     </r>
@@ -416,6 +444,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>size</t>
     </r>
@@ -424,6 +453,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>」をクリックすれば太さ順に色帯を並び変えることができます。</t>
     </r>
@@ -437,6 +467,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>(</t>
     </r>
@@ -445,6 +476,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>图表顶部或底部</t>
     </r>
@@ -453,6 +485,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>)</t>
     </r>
@@ -461,6 +494,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>上，您可了解到每个国家的难民申请人数，以及它在难民申请总人数中所占的比例。当您的鼠标移过色带，还可以看到按来源及目的地国统计的难民申请数量。您可以点击并拖拽国家名称，来调整国家顺序，也可以点击“来源国”旁的“</t>
     </r>
@@ -469,6 +503,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>alpha”</t>
     </r>
@@ -477,6 +512,7 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>或“</t>
     </r>
@@ -485,6 +521,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>size”</t>
     </r>
@@ -493,248 +530,203 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>字样，按照字母顺序或人数规模来进行排序。</t>
     </r>
   </si>
   <si>
-    <t>subtitle.timerange</t>
-  </si>
-  <si>
-    <t>Jan – Sept 2015</t>
-  </si>
-  <si>
-    <t>Janvier – septembre 2015: </t>
-  </si>
-  <si>
-    <t>subtitle.sum</t>
-  </si>
-  <si>
-    <t>995,190</t>
-  </si>
-  <si>
-    <t>995 190</t>
-  </si>
-  <si>
-    <t>subtitle.prepend</t>
-  </si>
-  <si>
-    <t>first time asylum applicants</t>
-  </si>
-  <si>
-    <t>demandeurs d'asile pour la première fois</t>
-  </si>
-  <si>
-    <t>Jan - Sept 2015: 807'965 Asylgesuche</t>
-  </si>
-  <si>
-    <t>Gennaio-Settembre 2015: 807'965 domande d'asilo</t>
-  </si>
-  <si>
-    <t>Janeiro a setembro de 2015: 807.965 pedidos de asilo político</t>
-  </si>
-  <si>
-    <r>
-      <t>يناير </t>
+    <t>subtitle</t>
+  </si>
+  <si>
+    <t>Jan – Sept 2015: 849,070 asylum applications</t>
+  </si>
+  <si>
+    <t>Janvier – septembre 2015: 849'070 demandes d'asile</t>
+  </si>
+  <si>
+    <t>Jan - Sept 2015: 849'070 Asylgesuche</t>
+  </si>
+  <si>
+    <t>Gennaio-Settembre 2015: 849'070 domande d'asilo</t>
+  </si>
+  <si>
+    <t>Janeiro a setembro de 2015: 849.070 pedidos de asilo político</t>
+  </si>
+  <si>
+    <t>يناير - سبتمبر 2015: 849070 مطلب لجوء</t>
+  </si>
+  <si>
+    <t>Январь-сентябрь 2015 года: общее число ходатайств о предоставлении убежища составило 849 070</t>
+  </si>
+  <si>
+    <t>ENE - SEP 2015; 849 070 solicitudes de asilo</t>
+  </si>
+  <si>
+    <t>２０１５年１月～９月の難民申請者数：８4 万 9 0 7 0人</t>
+  </si>
+  <si>
+    <r>
+      <t>2015</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>年</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t>- </t>
+        <charset val="1"/>
+      </rPr>
+      <t>1-9</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-      </rPr>
-      <t>سبتمبر </t>
+        <charset val="1"/>
+      </rPr>
+      <t>月：</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t>2015: 807965 </t>
+        <charset val="1"/>
+      </rPr>
+      <t>849'070</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-      </rPr>
-      <t>مطلب لجوء</t>
-    </r>
-  </si>
-  <si>
-    <t>Январь-сентябрь 2015 года: общее число ходатайств о предоставлении убежища составило 807 965</t>
-  </si>
-  <si>
-    <t>ENE - SEP 2015; 807 965 solicitudes de asilo</t>
-  </si>
-  <si>
-    <t>２０１５年１月～９月の難民申請者数：８０万７９６５人</t>
-  </si>
-  <si>
-    <r>
-      <t>2015</t>
+        <charset val="1"/>
+      </rPr>
+      <t>份难民申请</t>
+    </r>
+  </si>
+  <si>
+    <t>origins</t>
+  </si>
+  <si>
+    <t>Countries of origin</t>
+  </si>
+  <si>
+    <t>Pays d'origine</t>
+  </si>
+  <si>
+    <t>Herkunftsländer</t>
+  </si>
+  <si>
+    <t>Paesi di provenienza</t>
+  </si>
+  <si>
+    <t>Países de origem</t>
+  </si>
+  <si>
+    <t>بلدان المصدر</t>
+  </si>
+  <si>
+    <t>Страны, откуда прибывают беженцы</t>
+  </si>
+  <si>
+    <t>Países de origen</t>
+  </si>
+  <si>
+    <t>難民の出身国</t>
+  </si>
+  <si>
+    <t>来源国</t>
+  </si>
+  <si>
+    <t>destinations</t>
+  </si>
+  <si>
+    <t>Destination countries</t>
+  </si>
+  <si>
+    <t>Pays de destination</t>
+  </si>
+  <si>
+    <t>Zielländer</t>
+  </si>
+  <si>
+    <t>Paesi di destinazione</t>
+  </si>
+  <si>
+    <t>Países de destino</t>
+  </si>
+  <si>
+    <t>بلدان الوجهة </t>
+  </si>
+  <si>
+    <t>Страны, куда прибывают беженцы</t>
+  </si>
+  <si>
+    <t>難民の受け入れ国</t>
+  </si>
+  <si>
+    <t>目的地国</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Quelle</t>
+  </si>
+  <si>
+    <t>Fonte</t>
+  </si>
+  <si>
+    <t>fonte</t>
+  </si>
+  <si>
+    <t>المصدر</t>
+  </si>
+  <si>
+    <t>Источник:</t>
+  </si>
+  <si>
+    <t>Fuente</t>
+  </si>
+  <si>
+    <t>出典</t>
+  </si>
+  <si>
+    <t>来源</t>
+  </si>
+  <si>
+    <t>eurostat</t>
+  </si>
+  <si>
+    <t>Eurostat</t>
+  </si>
+  <si>
+    <t>مكتب الإحصاء بالإتحاد الأوروبي </t>
+  </si>
+  <si>
+    <t>Евростат</t>
+  </si>
+  <si>
+    <r>
+      <t>EU</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-      </rPr>
-      <t>年</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1-9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>月：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>807'965</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>份难民申请</t>
-    </r>
-  </si>
-  <si>
-    <t>origins</t>
-  </si>
-  <si>
-    <t>Countries of origin</t>
-  </si>
-  <si>
-    <t>Pays d'origine</t>
-  </si>
-  <si>
-    <t>Herkunftsländer</t>
-  </si>
-  <si>
-    <t>Paesi di provenienza</t>
-  </si>
-  <si>
-    <t>Países de origem</t>
-  </si>
-  <si>
-    <t>بلدان المصدر</t>
-  </si>
-  <si>
-    <t>Страны, откуда прибывают беженцы</t>
-  </si>
-  <si>
-    <t>Países de origen</t>
-  </si>
-  <si>
-    <t>難民の出身国</t>
-  </si>
-  <si>
-    <t>来源国</t>
-  </si>
-  <si>
-    <t>destinations</t>
-  </si>
-  <si>
-    <t>Destination countries</t>
-  </si>
-  <si>
-    <t>Pays de destination</t>
-  </si>
-  <si>
-    <t>Zielländer</t>
-  </si>
-  <si>
-    <t>Paesi di destinazione</t>
-  </si>
-  <si>
-    <t>Países de destino</t>
-  </si>
-  <si>
-    <t>بلدان الوجهة </t>
-  </si>
-  <si>
-    <t>Страны, куда прибывают беженцы</t>
-  </si>
-  <si>
-    <t>難民の受け入れ国</t>
-  </si>
-  <si>
-    <t>目的地国</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>Quelle</t>
-  </si>
-  <si>
-    <t>Fonte</t>
-  </si>
-  <si>
-    <t>fonte</t>
-  </si>
-  <si>
-    <t>المصدر</t>
-  </si>
-  <si>
-    <t>Источник:</t>
-  </si>
-  <si>
-    <t>Fuente</t>
-  </si>
-  <si>
-    <t>出典</t>
-  </si>
-  <si>
-    <t>来源</t>
-  </si>
-  <si>
-    <t>eurostat</t>
-  </si>
-  <si>
-    <t>Eurostat</t>
-  </si>
-  <si>
-    <t>مكتب الإحصاء بالإتحاد الأوروبي </t>
-  </si>
-  <si>
-    <t>Евростат</t>
-  </si>
-  <si>
-    <r>
-      <t>EU</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>統計局</t>
     </r>
@@ -1223,6 +1215,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1243,6 +1236,7 @@
       <sz val="10"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1293,7 +1287,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1307,6 +1301,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1327,10 +1325,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="19:19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1515,7 +1513,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="2" customFormat="true" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>55</v>
       </c>
@@ -1525,181 +1523,189 @@
       <c r="C6" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="2" t="n">
-        <v>995190</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>995190</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>995190</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>995190</v>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>995190</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>995190</v>
-      </c>
-      <c r="J7" s="2" t="n">
-        <v>995190</v>
-      </c>
-      <c r="K7" s="2" t="n">
-        <v>995190</v>
-      </c>
-    </row>
-    <row r="8" s="2" customFormat="true" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="J6" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="2" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="B7" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="C7" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="D7" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="E7" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="F7" s="0" t="s">
         <v>71</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="G11" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H11" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="J10" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K10" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
         <v>101</v>
       </c>
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -1718,609 +1724,571 @@
         <v>103</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>0</v>
+      <c r="J12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="K17" s="1" t="s">
         <v>140</v>
       </c>
+    </row>
+    <row r="17" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>148</v>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>218</v>
+        <v>233</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>225</v>
+        <v>244</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>243</v>
-      </c>
       <c r="C29" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="E30" s="0" t="s">
         <v>257</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="0" t="s">
-        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
before sending production versions
</commit_message>
<xml_diff>
--- a/input/translation_asylumFlowsEU.xlsx
+++ b/input/translation_asylumFlowsEU.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="translation_asylumFlowsEU" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="258">
   <si>
     <t>code</t>
   </si>
@@ -76,7 +76,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>- </t>
     </r>
@@ -85,7 +84,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>البلدان الأصلية والوجهات </t>
     </r>
@@ -108,7 +106,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>-</t>
     </r>
@@ -117,7 +114,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>来源国与目的地国</t>
     </r>
@@ -129,13 +125,13 @@
     <t>The ribbons' sizes are proportional to the number of asylum applications by country of origin and destination. Destination countries connected to countries of origin by thick ribbons have registered more asylum seekers than countries with thinner ribbons. </t>
   </si>
   <si>
-    <t>Les tailles des rubans sont proportionnelles au nombre de demandes d'asile selon le pays d'origine et de destination. Les pays de destination liés à des pays d'origine par un ruban épais ont enregistré davantage de demandes d'asile que les pays avec des rubans plus minces. </t>
+    <t>Les tailles des rubans sont proportionnelles au nombre de demandes d'asile par pays d'origine et de destination. Plus le ruban est épais, plus grand est le nombre de réfugiés que le pays a vu partir (en haut), respectivement arriver (en bas).</t>
   </si>
   <si>
     <t>Die Breite der Bänder zwischen Herkunfts- und Zielland ist proportional zur Anzahl migrierter Asylsuchender. Je breiter das Band, desto mehr migrierte Asylsuchende.</t>
   </si>
   <si>
-    <t>La dimensione delle bande è proporzionale al numero di domande d'asilo, secondo il paese d'origine e quello di destinazione. I paesi di destinazione legati ai paesi d'origine con bande più larghe hanno registrato un numero più alto di domande d'asilo rispetto ai paesi legati da bande più strette. </t>
+    <t>La dimensione delle bande è proporzionale al numero di domande d'asilo, secondo il paese d'origine e quello di destinazione. I paesi di destinazione legati ai paesi d'origine con bande più larghe hanno registrato un numero più alto di domande d'asilo rispetto ai paesi legati da bande più strette.</t>
   </si>
   <si>
     <t>Os tamanhos das faixas são proporcionais ao número de pedidos de asilo político por país de origem e destino. Países de destino ligados aos países de orgiem por faixas grossas registraram mais solicitantes de asilo do que países com faixas mais finas. </t>
@@ -149,7 +145,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>. </t>
     </r>
@@ -158,7 +153,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>حينما يكون الربط بين بلدان المقصد وبلدان المنشأ عن طريق شرائط سميكة، فذلك يعني أنها سجّلت توافد عدد أكبر من طالبي اللجوء مقارنة بالبلدان المرتبطة بشرائط أرقّ</t>
     </r>
@@ -167,7 +161,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>. </t>
     </r>
@@ -244,7 +237,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>. </t>
     </r>
@@ -253,7 +245,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>إذا كنت تنتقل عبر الدول </t>
     </r>
@@ -262,7 +253,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>(</t>
     </r>
@@ -271,7 +261,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>في الأعلى أو في الأسفل</t>
     </r>
@@ -280,7 +269,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>) </t>
     </r>
@@ -289,7 +277,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>بالفأرة، سترى إجمالي عدد طلبات اللجوء حسب البلد وما تمثله من نسبة مائوية من إجمالي الطلبات</t>
     </r>
@@ -298,7 +285,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>. </t>
     </r>
@@ -307,7 +293,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>إذا قمت بتحريك الفأرة فوق أحد الأشرطة، سترى عدد طلبات اللجوء حسب بلد المنشأ والمقصد</t>
     </r>
@@ -316,7 +301,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>. </t>
     </r>
@@ -325,7 +309,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>يُمكن أيضا إعادة ترتيب الدول من خلال النقر أو الإمساك أو السّحب</t>
     </r>
@@ -334,7 +317,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>. </t>
     </r>
@@ -343,7 +325,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>كما يُمكن إعادة ترتيبها أبجديا </t>
     </r>
@@ -352,7 +333,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>(</t>
     </r>
@@ -361,7 +341,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>عن طريق النقر على </t>
     </r>
@@ -370,7 +349,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>'alpha')</t>
     </r>
@@ -379,7 +357,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>، أو حسب الحجم </t>
     </r>
@@ -388,7 +365,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>(</t>
     </r>
@@ -397,7 +373,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>بالنقر على </t>
     </r>
@@ -406,7 +381,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>'size').</t>
     </r>
@@ -426,7 +400,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>alpha</t>
     </r>
@@ -435,7 +408,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>」をクリックするとアルファベット順に、「</t>
     </r>
@@ -444,7 +416,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>size</t>
     </r>
@@ -453,7 +424,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>」をクリックすれば太さ順に色帯を並び変えることができます。</t>
     </r>
@@ -467,7 +437,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>(</t>
     </r>
@@ -476,7 +445,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>图表顶部或底部</t>
     </r>
@@ -485,7 +453,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>)</t>
     </r>
@@ -494,7 +461,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>上，您可了解到每个国家的难民申请人数，以及它在难民申请总人数中所占的比例。当您的鼠标移过色带，还可以看到按来源及目的地国统计的难民申请数量。您可以点击并拖拽国家名称，来调整国家顺序，也可以点击“来源国”旁的“</t>
     </r>
@@ -503,7 +469,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>alpha”</t>
     </r>
@@ -512,7 +477,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>或“</t>
     </r>
@@ -521,7 +485,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>size”</t>
     </r>
@@ -530,7 +493,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>字样，按照字母顺序或人数规模来进行排序。</t>
     </r>
@@ -554,7 +516,41 @@
     <t>Janeiro a setembro de 2015: 849.070 pedidos de asilo político</t>
   </si>
   <si>
-    <t>يناير - سبتمبر 2015: 849070 مطلب لجوء</t>
+    <r>
+      <t>يناير </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>سبتمبر </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2015: 849070 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>مطلب لجوء</t>
+    </r>
   </si>
   <si>
     <t>Январь-сентябрь 2015 года: общее число ходатайств о предоставлении убежища составило 849 070</t>
@@ -563,7 +559,41 @@
     <t>ENE - SEP 2015; 849 070 solicitudes de asilo</t>
   </si>
   <si>
-    <t>２０１５年１月～９月の難民申請者数：８4 万 9 0 7 0人</t>
+    <r>
+      <t>２０１５年１月～９月の難民申請者数：８</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>万 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>9 0 7 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>人</t>
+    </r>
   </si>
   <si>
     <r>
@@ -574,7 +604,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>年</t>
     </r>
@@ -583,7 +612,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>1-9</t>
     </r>
@@ -592,7 +620,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>月：</t>
     </r>
@@ -601,7 +628,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>849'070</t>
     </r>
@@ -610,7 +636,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>份难民申请</t>
     </r>
@@ -726,7 +751,6 @@
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t>統計局</t>
     </r>
@@ -735,6 +759,9 @@
     <t>credit</t>
   </si>
   <si>
+    <t>Codice</t>
+  </si>
+  <si>
     <t>code.Afghanistan</t>
   </si>
   <si>
@@ -1198,9 +1225,6 @@
   </si>
   <si>
     <t>英国</t>
-  </si>
-  <si>
-    <t>Janvi – Sept 2015</t>
   </si>
 </sst>
 </file>
@@ -1210,12 +1234,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1233,10 +1256,15 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1296,15 +1324,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1325,51 +1353,51 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4438775510204"/>
-    <col collapsed="false" hidden="false" max="11" min="2" style="0" width="92.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="85.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="25.515306122449"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1392,7 +1420,7 @@
       <c r="F2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H2" s="0" t="s">
@@ -1401,10 +1429,10 @@
       <c r="I2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1427,7 +1455,7 @@
       <c r="F3" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H3" s="0" t="s">
@@ -1436,10 +1464,10 @@
       <c r="I3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1462,7 +1490,7 @@
       <c r="F4" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H4" s="0" t="s">
@@ -1471,10 +1499,10 @@
       <c r="I4" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="2" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1497,7 +1525,7 @@
       <c r="F5" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>50</v>
       </c>
       <c r="H5" s="0" t="s">
@@ -1506,45 +1534,45 @@
       <c r="I5" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" s="2" customFormat="true" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+    <row r="6" s="3" customFormat="true" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1567,7 +1595,7 @@
       <c r="F7" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>72</v>
       </c>
       <c r="H7" s="0" t="s">
@@ -1576,10 +1604,10 @@
       <c r="I7" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="2" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1602,7 +1630,7 @@
       <c r="F8" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>83</v>
       </c>
       <c r="H8" s="0" t="s">
@@ -1611,10 +1639,10 @@
       <c r="I8" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="2" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1637,7 +1665,7 @@
       <c r="F9" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>91</v>
       </c>
       <c r="H9" s="0" t="s">
@@ -1646,10 +1674,10 @@
       <c r="I9" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="2" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1672,7 +1700,7 @@
       <c r="F10" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="2" t="s">
         <v>98</v>
       </c>
       <c r="H10" s="0" t="s">
@@ -1688,606 +1716,591 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+    <row r="11" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="E11" s="3" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="G12" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="H12" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="J12" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="J12" s="2" t="s">
         <v>109</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>111</v>
-      </c>
       <c r="F13" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="G13" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="G13" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="H13" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="K13" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>118</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>120</v>
-      </c>
       <c r="E14" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="G14" s="1" t="s">
         <v>123</v>
       </c>
+      <c r="G14" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="H14" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="K14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>126</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>128</v>
-      </c>
       <c r="F15" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="I15" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="K15" s="1" t="s">
+      <c r="J15" s="2" t="s">
         <v>134</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="G16" s="1" t="s">
         <v>137</v>
       </c>
+      <c r="G16" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="H16" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="K16" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="17" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B17" s="2" t="s">
+    </row>
+    <row r="17" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
+      <c r="B17" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="G18" s="1" t="s">
         <v>149</v>
       </c>
+      <c r="G18" s="2" t="s">
+        <v>150</v>
+      </c>
       <c r="H18" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="J18" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="J18" s="2" t="s">
         <v>153</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F19" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="I19" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="K19" s="1" t="s">
+      <c r="J19" s="2" t="s">
         <v>163</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C20" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>165</v>
-      </c>
       <c r="F20" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="G20" s="1" t="s">
         <v>169</v>
       </c>
+      <c r="G20" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="H20" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="K20" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>172</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="G21" s="1" t="s">
         <v>179</v>
       </c>
+      <c r="G21" s="2" t="s">
+        <v>180</v>
+      </c>
       <c r="H21" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="J21" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="J21" s="2" t="s">
         <v>183</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="G22" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="G22" s="2" t="s">
+        <v>191</v>
+      </c>
       <c r="H22" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="J22" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="J22" s="2" t="s">
         <v>194</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F23" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="I23" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="K23" s="1" t="s">
+      <c r="J23" s="2" t="s">
         <v>203</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="G24" s="1" t="s">
         <v>210</v>
       </c>
+      <c r="G24" s="2" t="s">
+        <v>211</v>
+      </c>
       <c r="H24" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="J24" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="J24" s="2" t="s">
         <v>214</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F25" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="I25" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="K25" s="1" t="s">
+      <c r="J25" s="2" t="s">
         <v>224</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="G26" s="1" t="s">
         <v>231</v>
       </c>
+      <c r="G26" s="2" t="s">
+        <v>232</v>
+      </c>
       <c r="H26" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="J26" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="J26" s="2" t="s">
         <v>235</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="G27" s="1" t="s">
         <v>242</v>
       </c>
+      <c r="G27" s="2" t="s">
+        <v>243</v>
+      </c>
       <c r="H27" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="J27" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="J27" s="2" t="s">
         <v>246</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="G28" s="1" t="s">
         <v>253</v>
       </c>
+      <c r="G28" s="2" t="s">
+        <v>254</v>
+      </c>
       <c r="H28" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="K28" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="0" t="s">
+      <c r="K28" s="2" t="s">
         <v>257</v>
       </c>
     </row>

</xml_diff>